<commit_message>
cloud and crossbrowser demos
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdataprovider.xlsx
+++ b/src/test/resources/testdata/testdataprovider.xlsx
@@ -4,8 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="registrationData" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="registration" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="registration" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="products" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>USERNAME</t>
   </si>
@@ -121,6 +121,39 @@
   </si>
   <si>
     <t>xjohndoe3</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>jersey cotton striped polo shirt</t>
+  </si>
+  <si>
+    <t>baseball t-shirt</t>
+  </si>
+  <si>
+    <t>fruit of the loom</t>
+  </si>
+  <si>
+    <t>womens high heel point toe stiletto sandals</t>
+  </si>
+  <si>
+    <t>viva glam lipstick</t>
+  </si>
+  <si>
+    <t>flash bronzer body gel</t>
+  </si>
+  <si>
+    <t>shaving cream</t>
+  </si>
+  <si>
+    <t>obsession night perfume</t>
+  </si>
+  <si>
+    <t>curls to straight shampoo</t>
+  </si>
+  <si>
+    <t>paper towns</t>
   </si>
 </sst>
 </file>
@@ -162,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -175,14 +208,11 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,53 +533,133 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="5"/>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12345.0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3">
+        <v>12345.0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3">
+        <v>12345.0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -567,131 +677,58 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>3</v>
+      <c r="A3" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>